<commit_message>
attendacne at initial stage
</commit_message>
<xml_diff>
--- a/Hotel DB.xlsx
+++ b/Hotel DB.xlsx
@@ -294,9 +294,6 @@
     <t>OutTime</t>
   </si>
   <si>
-    <t>HoursWorked</t>
-  </si>
-  <si>
     <t>PaySlipID</t>
   </si>
   <si>
@@ -373,6 +370,9 @@
   </si>
   <si>
     <t>FloorID</t>
+  </si>
+  <si>
+    <t>AttendanceStatus</t>
   </si>
 </sst>
 </file>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +767,7 @@
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" customWidth="1"/>
     <col min="15" max="15" width="11.85546875" customWidth="1"/>
     <col min="16" max="16" width="15.140625" customWidth="1"/>
     <col min="17" max="17" width="12.5703125" customWidth="1"/>
@@ -780,7 +780,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>35</v>
@@ -819,16 +819,16 @@
         <v>72</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>11</v>
@@ -839,7 +839,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -878,19 +878,19 @@
         <v>73</v>
       </c>
       <c r="O2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -913,7 +913,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>3</v>
@@ -940,16 +940,16 @@
         <v>25</v>
       </c>
       <c r="P3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>111</v>
+      </c>
+      <c r="R3" t="s">
         <v>108</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>112</v>
-      </c>
-      <c r="R3" t="s">
-        <v>109</v>
-      </c>
-      <c r="S3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1002,10 +1002,10 @@
         <v>4</v>
       </c>
       <c r="Q4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S4" t="s">
         <v>4</v>
@@ -1058,13 +1058,13 @@
         <v>76</v>
       </c>
       <c r="P5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S5" t="s">
         <v>18</v>
@@ -1117,7 +1117,7 @@
         <v>18</v>
       </c>
       <c r="R6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1146,7 +1146,7 @@
         <v>12</v>
       </c>
       <c r="N7" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="O7" t="s">
         <v>37</v>
@@ -1180,10 +1180,10 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>29</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>28</v>
@@ -1238,7 +1238,7 @@
         <v>44</v>
       </c>
       <c r="O11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G13" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L13" t="s">
         <v>63</v>
@@ -1308,7 +1308,7 @@
         <v>12</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>12</v>
@@ -1325,7 +1325,7 @@
         <v>13</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="5" t="s">
@@ -1361,7 +1361,7 @@
         <v>15</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G25" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>

</xml_diff>

<commit_message>
Customer SC done UD remaining, Booking C initially done
</commit_message>
<xml_diff>
--- a/Hotel DB.xlsx
+++ b/Hotel DB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="123">
   <si>
     <t>Room</t>
   </si>
@@ -373,6 +373,18 @@
   </si>
   <si>
     <t>AttendanceStatus</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>cheque</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>OnlinePayment</t>
   </si>
 </sst>
 </file>
@@ -746,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="L20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +772,7 @@
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
@@ -1417,6 +1429,31 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L31" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L32" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L33" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L34" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add component error solved
</commit_message>
<xml_diff>
--- a/Hotel DB.xlsx
+++ b/Hotel DB.xlsx
@@ -764,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U34"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,11 +789,11 @@
     <col min="15" max="15" width="11.85546875" customWidth="1"/>
     <col min="16" max="16" width="15.140625" customWidth="1"/>
     <col min="17" max="17" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -836,26 +836,26 @@
       <c r="N1" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="O1" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="P1" s="4" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="U1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -898,26 +898,26 @@
       <c r="N2" t="s">
         <v>46</v>
       </c>
+      <c r="O2" t="s">
+        <v>73</v>
+      </c>
       <c r="P2" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="Q2" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="R2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="S2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T2" t="s">
-        <v>106</v>
-      </c>
-      <c r="U2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -960,26 +960,26 @@
       <c r="N3" t="s">
         <v>9</v>
       </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
       <c r="R3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="S3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="T3" t="s">
-        <v>108</v>
-      </c>
-      <c r="U3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1022,26 +1022,26 @@
       <c r="N4" t="s">
         <v>66</v>
       </c>
+      <c r="O4" t="s">
+        <v>74</v>
+      </c>
       <c r="P4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q4" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="R4" t="s">
+        <v>117</v>
+      </c>
+      <c r="S4" t="s">
+        <v>113</v>
+      </c>
+      <c r="T4" t="s">
         <v>4</v>
       </c>
-      <c r="S4" t="s">
-        <v>117</v>
-      </c>
-      <c r="T4" t="s">
-        <v>113</v>
-      </c>
-      <c r="U4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1084,26 +1084,26 @@
       <c r="N5" t="s">
         <v>47</v>
       </c>
+      <c r="O5" t="s">
+        <v>90</v>
+      </c>
       <c r="P5" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="Q5" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="R5" t="s">
         <v>116</v>
       </c>
       <c r="S5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="T5" t="s">
-        <v>110</v>
-      </c>
-      <c r="U5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1143,20 +1143,20 @@
       <c r="N6" t="s">
         <v>81</v>
       </c>
+      <c r="O6" t="s">
+        <v>91</v>
+      </c>
       <c r="P6" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="Q6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R6" t="s">
         <v>18</v>
       </c>
-      <c r="T6" t="s">
+      <c r="S6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1181,14 +1181,14 @@
       <c r="N7" t="s">
         <v>48</v>
       </c>
+      <c r="O7" t="s">
+        <v>118</v>
+      </c>
       <c r="P7" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1210,11 +1210,11 @@
       <c r="N8" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="P8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>95</v>
       </c>
@@ -1233,11 +1233,11 @@
       <c r="N9" t="s">
         <v>49</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="P9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -1256,11 +1256,11 @@
       <c r="N10" t="s">
         <v>51</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="P10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1273,11 +1273,11 @@
       <c r="N11" t="s">
         <v>57</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="P11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G12" s="2" t="s">
         <v>31</v>
       </c>
@@ -1287,11 +1287,11 @@
       <c r="N12" t="s">
         <v>58</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="P12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G13" s="2" t="s">
         <v>99</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G14" s="2" t="s">
         <v>29</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
         <v>33</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Made changes in servicehome
</commit_message>
<xml_diff>
--- a/Hotel DB.xlsx
+++ b/Hotel DB.xlsx
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Provided some page load checks
</commit_message>
<xml_diff>
--- a/Hotel DB.xlsx
+++ b/Hotel DB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="134">
   <si>
     <t>Room</t>
   </si>
@@ -391,6 +391,33 @@
   </si>
   <si>
     <t>ServiceTypeID</t>
+  </si>
+  <si>
+    <t>Booked</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>BillID</t>
+  </si>
+  <si>
+    <t>RoomCharges</t>
+  </si>
+  <si>
+    <t>ServiceCharges</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>DiscountedAmount</t>
+  </si>
+  <si>
+    <t>PaybleAmount</t>
+  </si>
+  <si>
+    <t>Details</t>
   </si>
 </sst>
 </file>
@@ -764,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +804,7 @@
     <col min="3" max="3" width="9.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
@@ -791,9 +818,10 @@
     <col min="17" max="17" width="12.5703125" customWidth="1"/>
     <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -854,8 +882,11 @@
       <c r="T1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -916,8 +947,11 @@
       <c r="T2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -978,8 +1012,11 @@
       <c r="T3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1040,8 +1077,11 @@
       <c r="T4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1102,8 +1142,11 @@
       <c r="T5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1155,8 +1198,11 @@
       <c r="S6" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1187,8 +1233,11 @@
       <c r="P7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1213,8 +1262,11 @@
       <c r="P8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>95</v>
       </c>
@@ -1236,8 +1288,11 @@
       <c r="P9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -1259,8 +1314,11 @@
       <c r="P10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1277,7 +1335,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G12" s="2" t="s">
         <v>31</v>
       </c>
@@ -1291,7 +1349,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G13" s="2" t="s">
         <v>99</v>
       </c>
@@ -1299,7 +1357,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G14" s="2" t="s">
         <v>29</v>
       </c>
@@ -1307,7 +1365,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
         <v>33</v>
       </c>
@@ -1315,7 +1373,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
         <v>18</v>
       </c>
@@ -1409,6 +1467,9 @@
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F25" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="G25" s="5" t="s">
         <v>102</v>
       </c>

</xml_diff>